<commit_message>
update some fucking documents
</commit_message>
<xml_diff>
--- a/DesignFile/MIPS-55instr.xlsx
+++ b/DesignFile/MIPS-55instr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Code\ModelSim\Project1\P1-SRC\DesignFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45291FC-F0DF-4C27-A963-FC049C3880AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41CE1B5-20B6-4D13-99F1-D6D41E1E061B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{102853C8-9FF7-42E1-AA3E-8C2E021BEA53}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="221">
   <si>
     <t>R-Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -868,10 +868,6 @@
   </si>
   <si>
     <t>10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1516,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453AE6C8-F289-4297-9E64-55AC18882332}">
   <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19:S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2357,7 +2353,15 @@
       <c r="J19" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
       <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
@@ -2387,12 +2391,19 @@
       <c r="J20" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
       <c r="M20" s="31" t="s">
         <v>215</v>
       </c>
       <c r="N20" s="31" t="s">
         <v>220</v>
       </c>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
@@ -3341,8 +3352,8 @@
       <c r="M51" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="N51" s="1" t="s">
-        <v>221</v>
+      <c r="N51" s="31" t="s">
+        <v>217</v>
       </c>
       <c r="O51" s="31" t="s">
         <v>216</v>
@@ -3387,8 +3398,8 @@
       <c r="M52" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="N52" s="1" t="s">
-        <v>221</v>
+      <c r="N52" s="31" t="s">
+        <v>217</v>
       </c>
       <c r="O52" s="31" t="s">
         <v>216</v>
@@ -3433,8 +3444,8 @@
       <c r="M53" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="N53" s="1" t="s">
-        <v>221</v>
+      <c r="N53" s="31" t="s">
+        <v>217</v>
       </c>
       <c r="O53" s="31" t="s">
         <v>216</v>
@@ -3479,8 +3490,8 @@
       <c r="M54" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="N54" s="1" t="s">
-        <v>221</v>
+      <c r="N54" s="31" t="s">
+        <v>217</v>
       </c>
       <c r="O54" s="31" t="s">
         <v>216</v>
@@ -3525,8 +3536,8 @@
       <c r="M55" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="N55" s="1" t="s">
-        <v>221</v>
+      <c r="N55" s="31" t="s">
+        <v>217</v>
       </c>
       <c r="O55" s="31" t="s">
         <v>216</v>

</xml_diff>